<commit_message>
final changes to dotter 1
</commit_message>
<xml_diff>
--- a/examples/cases/example_02/Deltabeek.xlsx
+++ b/examples/cases/example_02/Deltabeek.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F3" sqref="F3:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G2">
         <v>0.1</v>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G3">
         <v>0.1</v>
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G4">
         <v>0.1</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G5">
         <v>0.1</v>
@@ -549,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G6">
         <v>0.1</v>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G7">
         <v>0.1</v>
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G8">
         <v>0.1</v>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G9">
         <v>0.1</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G10">
         <v>0.1</v>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G11">
         <v>0.1</v>
@@ -715,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G12">
         <v>0.1</v>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G13">
         <v>0.1</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G14">
         <v>0.1</v>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G15">
         <v>0.1</v>

</xml_diff>